<commit_message>
Copy Files From Source Repo (2026-01-23 09:33)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/tfrink_microsoft_com/Documents/Documents/BUSS/Learn courses/MS-4004 - V2 Mar 2025/Source docs/LP2-Empower your workforce with M365 use cases/M4-Marketing use case/track changes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/tfrink_microsoft_com/Documents/MS-4004 lab files/Reused files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <r>
       <rPr>
@@ -58,7 +58,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Artisanal Chai の売上 (ユニット数)</t>
+      <t>Artisanal Chai の販売 (ユニット数)</t>
     </r>
   </si>
   <si>
@@ -249,7 +249,18 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>4:36</t>
+      <t>3:15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>5:48</t>
     </r>
   </si>
   <si>
@@ -378,29 +389,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="none"/>
-        <strike val="0"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <color theme="1"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
@@ -415,6 +403,29 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <strike val="0"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -572,12 +583,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="1" headerRowBorderDxfId="2">
   <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Month" dataDxfId="1"/>
+    <tableColumn id="1" name="Month" dataDxfId="0"/>
     <tableColumn id="2" name="チャイの売上合計 (ユニット数)"/>
-    <tableColumn id="3" name="Artisanal Chai の売上 (ユニット数)"/>
+    <tableColumn id="3" name="Artisanal Chai の販売 (ユニット数)"/>
     <tableColumn id="4" name="事前に作成されたチャイの売上 (ユニット数)"/>
     <tableColumn id="5" name="ソーシャル メディア エンゲージメント (ビュー)"/>
     <tableColumn id="6" name="チャイのオンライン検索"/>
@@ -983,11 +994,11 @@
       <c r="C5">
         <v>499</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
+      <c r="D5">
+        <v>436</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>2996</v>
@@ -1001,11 +1012,11 @@
         <f t="shared" si="0"/>
         <v>863</v>
       </c>
-      <c r="C6">
-        <v>315</v>
-      </c>
-      <c r="D6">
-        <v>548</v>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
       <c r="E6">
         <v>3599</v>

</xml_diff>